<commit_message>
Qr code finalized to created from excel sheet.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabin\Desktop\QR-Code-Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F0C3E7D0-5D92-4D2F-BBDF-4A89F0A58B8B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D05DAA17-9CDC-4434-8851-C956704B98B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5760" xr2:uid="{4C628CDA-66BC-4364-BD7D-A6B212230E10}"/>
   </bookViews>
@@ -25,21 +25,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="9">
   <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>mobile</t>
-  </si>
-  <si>
-    <t>dob</t>
   </si>
   <si>
     <t>Prabin Siwakoti</t>
   </si>
   <si>
-    <t>Prabesh Siwakoti</t>
+    <t>school_name</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>Online Multimedia</t>
+  </si>
+  <si>
+    <t>photo_id</t>
+  </si>
+  <si>
+    <t>Prabesh</t>
+  </si>
+  <si>
+    <t>Shramik Nakarmi</t>
+  </si>
+  <si>
+    <t>Bibek Mahajan</t>
   </si>
 </sst>
 </file>
@@ -392,49 +404,1433 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAF1AE4-CA17-48CC-B2E7-0CC4A0DED7BD}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="G96" sqref="G96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>9842786501</v>
-      </c>
-      <c r="C2" s="1">
-        <v>55323</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>9804932008</v>
-      </c>
-      <c r="C3" s="1">
-        <v>63555</v>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s">
+        <v>4</v>
+      </c>
+      <c r="D94">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96">
+        <v>9842786501</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97">
+        <v>9804932009</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" t="s">
+        <v>4</v>
+      </c>
+      <c r="D98">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" t="s">
+        <v>4</v>
+      </c>
+      <c r="D99">
+        <v>98737373</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" t="s">
+        <v>4</v>
+      </c>
+      <c r="D100">
+        <v>1929929</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>8</v>
+      </c>
+      <c r="C101" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101">
+        <v>98737373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>